<commit_message>
catalog data fix, change readme
</commit_message>
<xml_diff>
--- a/app/api/catalog/catalog.xlsx
+++ b/app/api/catalog/catalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\DEV\snupia_utils\snupia_utils_front\app\api\catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D03FA9E-5AE8-4F04-AB6A-48872E12AE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A679F3-20B5-4BF1-AD85-4901757806CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2566" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2566" uniqueCount="911">
   <si>
     <t>title</t>
   </si>
@@ -28828,6 +28828,10 @@
   </si>
   <si>
     <t>Eight Concert Études op.40 piano solo - Prelude / Reverie / Toccatina / Reminiscence / Raillery / Pastoral / Intermezzo / Finale</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>임희준</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -29499,7 +29503,7 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="20">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -29661,22 +29665,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8ED873"/>
-          <bgColor rgb="FF8ED873"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF9999"/>
-          <bgColor rgb="FFFF9999"/>
         </patternFill>
       </fill>
     </dxf>
@@ -30996,8 +30984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A204" sqref="A1:A204"/>
+    <sheetView tabSelected="1" topLeftCell="L151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P177" sqref="P177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -37746,9 +37734,7 @@
       <c r="M152" s="35">
         <v>3</v>
       </c>
-      <c r="N152" s="28" t="s">
-        <v>646</v>
-      </c>
+      <c r="N152" s="28"/>
       <c r="O152" s="34"/>
       <c r="P152" s="28" t="s">
         <v>413</v>
@@ -37791,7 +37777,9 @@
       <c r="M153" s="35">
         <v>3</v>
       </c>
-      <c r="N153" s="28"/>
+      <c r="N153" s="50" t="s">
+        <v>910</v>
+      </c>
       <c r="O153" s="34"/>
       <c r="P153" s="28" t="s">
         <v>417</v>
@@ -38766,7 +38754,7 @@
       </c>
       <c r="O175" s="34"/>
       <c r="P175" s="28" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="Q175" s="28"/>
       <c r="R175" s="28" t="s">
@@ -38811,7 +38799,7 @@
       <c r="N176" s="28"/>
       <c r="O176" s="34"/>
       <c r="P176" s="28" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="Q176" s="28"/>
       <c r="R176" s="28" t="s">
@@ -40850,40 +40838,40 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A3:A204">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>NOT(AND(B3&lt;&gt;"", M3&lt;&gt;""))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>AND(B3&lt;&gt;"", M3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A182:A183">
-    <cfRule type="expression" dxfId="21" priority="11">
+    <cfRule type="expression" dxfId="17" priority="11">
       <formula>NOT(AND(C182&lt;&gt;"", M182&lt;&gt;""))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="12">
+    <cfRule type="expression" dxfId="16" priority="12">
       <formula>AND(C182&lt;&gt;"", M182&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J204">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M204">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -52285,40 +52273,40 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A3:A181 A183:A202">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>NOT(AND(B3&lt;&gt;"", M3&lt;&gt;""))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>AND(B3&lt;&gt;"", M3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A182">
-    <cfRule type="expression" dxfId="17" priority="9">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>NOT(AND(C182&lt;&gt;"", M182&lt;&gt;""))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="10">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>AND(C182&lt;&gt;"", M182&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:J202">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M202">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>